<commit_message>
Added size scenario array
</commit_message>
<xml_diff>
--- a/docs/Files/ODYM_Classifications_Master_Vehicle_System.xlsx
+++ b/docs/Files/ODYM_Classifications_Master_Vehicle_System.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6B6BB4-7198-D043-BFF2-D07DC7360CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31686DB8-5605-0C42-9F05-21FC1E3C5A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26680" yWindow="500" windowWidth="24520" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="MAIN_Table" sheetId="1" r:id="rId2"/>
     <sheet name="Energy_Storage_Scenarios" sheetId="39" r:id="rId3"/>
     <sheet name="Day" sheetId="38" r:id="rId4"/>
-    <sheet name="Ownership_Scenarios" sheetId="37" r:id="rId5"/>
+    <sheet name="Sieze_Scenarios" sheetId="37" r:id="rId5"/>
     <sheet name="Reuse_Scenarios" sheetId="36" r:id="rId6"/>
     <sheet name="Stock_Scenarios" sheetId="35" r:id="rId7"/>
     <sheet name="Size" sheetId="34" r:id="rId8"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="393">
   <si>
     <t>Name</t>
   </si>
@@ -994,9 +994,6 @@
     <t>Large</t>
   </si>
   <si>
-    <t>BAU</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -1051,9 +1048,6 @@
     <t>Graphite</t>
   </si>
   <si>
-    <t>Ownership_Scenarios</t>
-  </si>
-  <si>
     <t>Direct recycling</t>
   </si>
   <si>
@@ -1238,6 +1232,18 @@
   </si>
   <si>
     <t>Li_free</t>
+  </si>
+  <si>
+    <t>Size_Scenarios</t>
+  </si>
+  <si>
+    <t>Scenarios for vehicle size development</t>
+  </si>
+  <si>
+    <t>Shift to small cars</t>
+  </si>
+  <si>
+    <t>Shift to large cars</t>
   </si>
 </sst>
 </file>
@@ -12420,7 +12426,7 @@
         <v>234</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -13524,7 +13530,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -13539,7 +13545,7 @@
         <v>252</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -13554,7 +13560,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -13569,7 +13575,7 @@
         <v>237</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -13584,7 +13590,7 @@
         <v>43887</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -13599,7 +13605,7 @@
         <v>43887</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -14528,7 +14534,7 @@
         <v>43028</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -14577,7 +14583,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="D10" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -14618,7 +14624,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D15" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -14626,7 +14632,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D16" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -14634,7 +14640,7 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D17" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -15189,7 +15195,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -15393,10 +15399,10 @@
   <dimension ref="A1:AF1311"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="M7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15475,9 +15481,8 @@
         <f>Reuse_Scenarios!B1</f>
         <v>Reuse_Scenarios</v>
       </c>
-      <c r="R1" s="7" t="str">
-        <f>Ownership_Scenarios!B1</f>
-        <v>Ownership_Scenarios</v>
+      <c r="R1" s="7" t="s">
+        <v>389</v>
       </c>
       <c r="S1" s="7" t="str">
         <f>Day!B1</f>
@@ -15560,7 +15565,7 @@
         <v>Material</v>
       </c>
       <c r="R2" s="7" t="str">
-        <f>Ownership_Scenarios!B2</f>
+        <f>Sieze_Scenarios!B2</f>
         <v>Material</v>
       </c>
       <c r="S2" s="7" t="str">
@@ -15629,8 +15634,8 @@
         <v>Scenarios for chemistry development</v>
       </c>
       <c r="R3" s="7" t="str">
-        <f>Ownership_Scenarios!B3</f>
-        <v>Scenarios for chemistry development</v>
+        <f>Sieze_Scenarios!B3</f>
+        <v>Scenarios for vehicle size development</v>
       </c>
       <c r="S3" s="7" t="str">
         <f>Day!B3</f>
@@ -15698,7 +15703,7 @@
         <v>None</v>
       </c>
       <c r="R4" s="7" t="str">
-        <f>Ownership_Scenarios!B4</f>
+        <f>Sieze_Scenarios!B4</f>
         <v>None</v>
       </c>
       <c r="S4" s="7" t="str">
@@ -15767,7 +15772,7 @@
         <v>44694a9e-5884-11ea-8e2d-0242ac130003</v>
       </c>
       <c r="R5" s="7" t="str">
-        <f>Ownership_Scenarios!B5</f>
+        <f>Sieze_Scenarios!B5</f>
         <v>44694a9e-5884-11ea-8e2d-0242ac130003</v>
       </c>
       <c r="S5" s="7" t="str">
@@ -16149,15 +16154,15 @@
         <v>Small</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q11" s="7" t="str">
         <f>Reuse_Scenarios!D2</f>
         <v>LFP reused</v>
       </c>
       <c r="R11" s="7" t="str">
-        <f>Ownership_Scenarios!D2</f>
-        <v>Low</v>
+        <f>Sieze_Scenarios!D2</f>
+        <v>Shift to small cars</v>
       </c>
       <c r="S11" s="14" t="str">
         <f>Day!D2</f>
@@ -16228,8 +16233,8 @@
         <v>Direct recycling</v>
       </c>
       <c r="R12" s="7" t="str">
-        <f>Ownership_Scenarios!D3</f>
-        <v>BAU</v>
+        <f>Sieze_Scenarios!D3</f>
+        <v>Constant</v>
       </c>
       <c r="S12" s="14" t="str">
         <f>Day!D3</f>
@@ -16289,15 +16294,15 @@
         <v>Large</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q13" s="7" t="str">
         <f>Reuse_Scenarios!D4</f>
         <v>All reused</v>
       </c>
       <c r="R13" s="7" t="str">
-        <f>Ownership_Scenarios!D4</f>
-        <v>High</v>
+        <f>Sieze_Scenarios!D4</f>
+        <v>Shift to large cars</v>
       </c>
       <c r="S13" s="14" t="str">
         <f>Day!D4</f>
@@ -16398,7 +16403,7 @@
         <v>NCM523</v>
       </c>
       <c r="J16" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K16" s="7" t="str">
         <f>Segment!D7</f>
@@ -16427,7 +16432,7 @@
         <v>NCM622</v>
       </c>
       <c r="J17" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K17" s="7" t="str">
         <f>Segment!D8</f>
@@ -16456,7 +16461,7 @@
         <v>NCM622-Graphite (Si)</v>
       </c>
       <c r="J18" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="K18" s="7" t="str">
         <f>Segment!D9</f>
@@ -16485,7 +16490,7 @@
         <v>NCM712-Graphite (Si)</v>
       </c>
       <c r="J19" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K19" s="7" t="str">
         <f>Segment!D10</f>
@@ -16664,7 +16669,7 @@
         <v>S</v>
       </c>
       <c r="I27" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="S27" s="14" t="str">
         <f>Day!D18</f>
@@ -28753,7 +28758,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>9</v>
@@ -28773,7 +28778,7 @@
         <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -28787,7 +28792,7 @@
         <v>303</v>
       </c>
       <c r="D3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -28866,7 +28871,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6" t="s">
@@ -28885,10 +28890,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>330</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>332</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -28899,10 +28904,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>331</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>333</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -28916,7 +28921,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -28930,7 +28935,7 @@
         <v>236</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -28944,7 +28949,7 @@
         <v>43887</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -28958,7 +28963,7 @@
         <v>43887</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -28972,7 +28977,7 @@
         <v>234</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -28986,7 +28991,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -28995,7 +29000,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="D10" s="13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -29003,7 +29008,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D11" s="13" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -29011,7 +29016,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D12" s="13" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -29019,7 +29024,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D13" s="13" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -29027,7 +29032,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" s="13" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E14">
         <v>12</v>
@@ -29035,7 +29040,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D15" s="13" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -29043,7 +29048,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D16" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -29051,7 +29056,7 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D17" s="13" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -29059,7 +29064,7 @@
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D18" s="13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -29067,7 +29072,7 @@
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D19" s="13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E19">
         <v>17</v>
@@ -29075,7 +29080,7 @@
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D20" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E20">
         <v>18</v>
@@ -29083,7 +29088,7 @@
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D21" s="13" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E21">
         <v>19</v>
@@ -29091,7 +29096,7 @@
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D22" s="13" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E22">
         <v>20</v>
@@ -29099,7 +29104,7 @@
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D23" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E23">
         <v>21</v>
@@ -29107,7 +29112,7 @@
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D24" s="13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E24">
         <v>22</v>
@@ -29115,7 +29120,7 @@
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25" s="13" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E25">
         <v>23</v>
@@ -29123,7 +29128,7 @@
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26" s="13" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E26">
         <v>24</v>
@@ -29131,7 +29136,7 @@
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E27">
         <v>25</v>
@@ -29139,7 +29144,7 @@
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D28" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E28">
         <v>26</v>
@@ -29147,7 +29152,7 @@
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" s="13" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E29">
         <v>27</v>
@@ -29155,7 +29160,7 @@
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E30">
         <v>28</v>
@@ -29163,7 +29168,7 @@
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D31" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E31">
         <v>29</v>
@@ -29171,7 +29176,7 @@
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D32" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E32">
         <v>30</v>
@@ -29179,7 +29184,7 @@
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E33">
         <v>31</v>
@@ -29187,7 +29192,7 @@
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E34">
         <v>32</v>
@@ -29195,7 +29200,7 @@
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E35">
         <v>33</v>
@@ -29203,7 +29208,7 @@
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E36">
         <v>34</v>
@@ -29211,7 +29216,7 @@
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D37" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E37">
         <v>35</v>
@@ -29219,7 +29224,7 @@
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D38" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E38">
         <v>36</v>
@@ -29227,7 +29232,7 @@
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D39" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E39">
         <v>37</v>
@@ -29235,7 +29240,7 @@
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D40" s="13" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E40">
         <v>38</v>
@@ -29243,7 +29248,7 @@
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D41" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E41">
         <v>39</v>
@@ -29251,7 +29256,7 @@
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D42" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -29259,7 +29264,7 @@
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D43" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E43">
         <v>41</v>
@@ -29267,7 +29272,7 @@
     </row>
     <row r="44" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D44" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E44">
         <v>42</v>
@@ -29275,7 +29280,7 @@
     </row>
     <row r="45" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D45" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E45">
         <v>43</v>
@@ -29283,7 +29288,7 @@
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D46" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E46">
         <v>44</v>
@@ -29291,7 +29296,7 @@
     </row>
     <row r="47" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D47" s="13" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E47">
         <v>45</v>
@@ -29299,7 +29304,7 @@
     </row>
     <row r="48" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D48" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E48">
         <v>46</v>
@@ -29307,7 +29312,7 @@
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D49" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E49">
         <v>47</v>
@@ -29323,7 +29328,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29336,7 +29341,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>328</v>
+        <v>389</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>9</v>
@@ -29356,7 +29361,7 @@
         <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>311</v>
+        <v>391</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -29367,10 +29372,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>303</v>
+        <v>390</v>
       </c>
       <c r="D3" t="s">
-        <v>309</v>
+        <v>383</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -29384,7 +29389,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>310</v>
+        <v>392</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -29454,7 +29459,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>9</v>
@@ -29474,7 +29479,7 @@
         <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -29488,7 +29493,7 @@
         <v>303</v>
       </c>
       <c r="D3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -29502,7 +29507,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -29572,7 +29577,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>9</v>
@@ -29592,7 +29597,7 @@
         <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -29620,7 +29625,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -29866,7 +29871,7 @@
         <v>236</v>
       </c>
       <c r="D5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -29880,7 +29885,7 @@
         <v>43887</v>
       </c>
       <c r="D6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E6">
         <v>4</v>

</xml_diff>

<commit_message>
Deleted roskill, added all_LFP
</commit_message>
<xml_diff>
--- a/docs/Files/ODYM_Classifications_Master_Vehicle_System.xlsx
+++ b/docs/Files/ODYM_Classifications_Master_Vehicle_System.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31686DB8-5605-0C42-9F05-21FC1E3C5A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FBD012-6E86-7240-A8A6-1C9BFEBB81D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26680" yWindow="500" windowWidth="24520" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover_Dimensions_Aspects" sheetId="8" r:id="rId1"/>
@@ -1021,9 +1021,6 @@
     <t>GLOBAL</t>
   </si>
   <si>
-    <t>Roskill</t>
-  </si>
-  <si>
     <t>LNO</t>
   </si>
   <si>
@@ -1244,6 +1241,9 @@
   </si>
   <si>
     <t>Shift to large cars</t>
+  </si>
+  <si>
+    <t>All_LFP</t>
   </si>
 </sst>
 </file>
@@ -12426,7 +12426,7 @@
         <v>234</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -14534,7 +14534,7 @@
         <v>43028</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -14583,7 +14583,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="D10" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -14624,7 +14624,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D15" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -14632,7 +14632,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D16" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -14640,7 +14640,7 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D17" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -15195,7 +15195,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -15399,10 +15399,10 @@
   <dimension ref="A1:AF1311"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="M7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="O24" sqref="O24"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15482,7 +15482,7 @@
         <v>Reuse_Scenarios</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="S1" s="7" t="str">
         <f>Day!B1</f>
@@ -16336,7 +16336,7 @@
       </c>
       <c r="J14" t="str">
         <f>Chemistry_Scenarios!D5</f>
-        <v>Roskill</v>
+        <v>Constant</v>
       </c>
       <c r="K14" s="7" t="str">
         <f>Segment!D5</f>
@@ -16370,7 +16370,7 @@
       </c>
       <c r="J15" t="str">
         <f>Chemistry_Scenarios!D6</f>
-        <v>Constant</v>
+        <v>Faraday</v>
       </c>
       <c r="K15" s="7" t="str">
         <f>Segment!D6</f>
@@ -16402,8 +16402,9 @@
         <f>Battery_Chemistry!D7</f>
         <v>NCM523</v>
       </c>
-      <c r="J16" t="s">
-        <v>384</v>
+      <c r="J16" t="str">
+        <f>Chemistry_Scenarios!D7</f>
+        <v>BNEF</v>
       </c>
       <c r="K16" s="7" t="str">
         <f>Segment!D7</f>
@@ -16431,8 +16432,9 @@
         <f>Battery_Chemistry!D8</f>
         <v>NCM622</v>
       </c>
-      <c r="J17" t="s">
-        <v>385</v>
+      <c r="J17" t="str">
+        <f>Chemistry_Scenarios!D8</f>
+        <v>Next_gen_BNEF</v>
       </c>
       <c r="K17" s="7" t="str">
         <f>Segment!D8</f>
@@ -16460,8 +16462,9 @@
         <f>Battery_Chemistry!D9</f>
         <v>NCM622-Graphite (Si)</v>
       </c>
-      <c r="J18" t="s">
-        <v>387</v>
+      <c r="J18" t="str">
+        <f>Chemistry_Scenarios!D9</f>
+        <v>Li_free</v>
       </c>
       <c r="K18" s="7" t="str">
         <f>Segment!D9</f>
@@ -16489,8 +16492,9 @@
         <f>Battery_Chemistry!D10</f>
         <v>NCM712-Graphite (Si)</v>
       </c>
-      <c r="J19" t="s">
-        <v>388</v>
+      <c r="J19" t="str">
+        <f>Chemistry_Scenarios!D10</f>
+        <v>All_LFP</v>
       </c>
       <c r="K19" s="7" t="str">
         <f>Segment!D10</f>
@@ -16669,7 +16673,7 @@
         <v>S</v>
       </c>
       <c r="I27" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S27" s="14" t="str">
         <f>Day!D18</f>
@@ -28758,7 +28762,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>9</v>
@@ -28778,7 +28782,7 @@
         <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -28792,7 +28796,7 @@
         <v>303</v>
       </c>
       <c r="D3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -28871,7 +28875,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6" t="s">
@@ -28890,10 +28894,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -28904,10 +28908,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -28921,7 +28925,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -28935,7 +28939,7 @@
         <v>236</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -28949,7 +28953,7 @@
         <v>43887</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -28963,7 +28967,7 @@
         <v>43887</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -28977,7 +28981,7 @@
         <v>234</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -28991,7 +28995,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -29000,7 +29004,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="D10" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -29008,7 +29012,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D11" s="13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -29016,7 +29020,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D12" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -29024,7 +29028,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D13" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -29032,7 +29036,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E14">
         <v>12</v>
@@ -29040,7 +29044,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D15" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -29048,7 +29052,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D16" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -29056,7 +29060,7 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D17" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -29064,7 +29068,7 @@
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D18" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -29072,7 +29076,7 @@
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D19" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E19">
         <v>17</v>
@@ -29080,7 +29084,7 @@
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D20" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E20">
         <v>18</v>
@@ -29088,7 +29092,7 @@
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D21" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E21">
         <v>19</v>
@@ -29096,7 +29100,7 @@
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D22" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E22">
         <v>20</v>
@@ -29104,7 +29108,7 @@
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D23" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E23">
         <v>21</v>
@@ -29112,7 +29116,7 @@
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D24" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E24">
         <v>22</v>
@@ -29120,7 +29124,7 @@
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E25">
         <v>23</v>
@@ -29128,7 +29132,7 @@
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E26">
         <v>24</v>
@@ -29136,7 +29140,7 @@
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E27">
         <v>25</v>
@@ -29144,7 +29148,7 @@
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D28" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E28">
         <v>26</v>
@@ -29152,7 +29156,7 @@
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E29">
         <v>27</v>
@@ -29160,7 +29164,7 @@
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E30">
         <v>28</v>
@@ -29168,7 +29172,7 @@
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D31" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E31">
         <v>29</v>
@@ -29176,7 +29180,7 @@
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D32" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E32">
         <v>30</v>
@@ -29184,7 +29188,7 @@
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E33">
         <v>31</v>
@@ -29192,7 +29196,7 @@
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E34">
         <v>32</v>
@@ -29200,7 +29204,7 @@
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E35">
         <v>33</v>
@@ -29208,7 +29212,7 @@
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E36">
         <v>34</v>
@@ -29216,7 +29220,7 @@
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D37" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E37">
         <v>35</v>
@@ -29224,7 +29228,7 @@
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D38" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E38">
         <v>36</v>
@@ -29232,7 +29236,7 @@
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D39" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E39">
         <v>37</v>
@@ -29240,7 +29244,7 @@
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D40" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E40">
         <v>38</v>
@@ -29248,7 +29252,7 @@
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D41" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E41">
         <v>39</v>
@@ -29256,7 +29260,7 @@
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D42" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -29264,7 +29268,7 @@
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D43" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E43">
         <v>41</v>
@@ -29272,7 +29276,7 @@
     </row>
     <row r="44" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D44" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E44">
         <v>42</v>
@@ -29280,7 +29284,7 @@
     </row>
     <row r="45" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D45" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E45">
         <v>43</v>
@@ -29288,7 +29292,7 @@
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D46" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E46">
         <v>44</v>
@@ -29296,7 +29300,7 @@
     </row>
     <row r="47" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D47" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E47">
         <v>45</v>
@@ -29304,7 +29308,7 @@
     </row>
     <row r="48" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D48" s="13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E48">
         <v>46</v>
@@ -29312,7 +29316,7 @@
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D49" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E49">
         <v>47</v>
@@ -29341,7 +29345,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>9</v>
@@ -29361,7 +29365,7 @@
         <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -29372,10 +29376,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -29389,7 +29393,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -29459,7 +29463,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>9</v>
@@ -29479,7 +29483,7 @@
         <v>220</v>
       </c>
       <c r="D2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -29493,7 +29497,7 @@
         <v>303</v>
       </c>
       <c r="D3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -29507,7 +29511,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -29792,10 +29796,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7565329B-3E71-C64E-B679-B7780FD32074}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29871,7 +29875,7 @@
         <v>236</v>
       </c>
       <c r="D5" t="s">
-        <v>318</v>
+        <v>382</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -29898,6 +29902,12 @@
       <c r="B7" s="2">
         <v>43887</v>
       </c>
+      <c r="D7" t="s">
+        <v>384</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -29906,12 +29916,32 @@
       <c r="B8" t="s">
         <v>234</v>
       </c>
+      <c r="D8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>387</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E10">
         <v>8</v>
       </c>
     </row>

</xml_diff>